<commit_message>
export uraian jabatan excel
</commit_message>
<xml_diff>
--- a/public/template/Template_Dirjab.xlsx
+++ b/public/template/Template_Dirjab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\DIRJAB-IP\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C25C5-F999-4C08-ACFA-96F15235E62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA6411E-0D70-467E-AED9-B766073B7613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
-    <t>URAIAN JABATAN</t>
-  </si>
-  <si>
     <t>Tanggal</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>Sudah divalidasi</t>
+  </si>
+  <si>
+    <t>TEMPLATE JABATAN</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -446,6 +446,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,15 +502,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -478,44 +513,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -947,226 +944,226 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="30"/>
+      <c r="G7" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="43"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="B10" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-    </row>
-    <row r="12" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
+      <c r="B22" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
@@ -1179,54 +1176,54 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="C26" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="38"/>
+      <c r="H26" s="28"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="39">
+      <c r="B27" s="22">
         <v>1</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="H27" s="41"/>
+      <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28"/>
@@ -1302,37 +1299,37 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="H55" s="38"/>
+      <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E56"/>
@@ -1362,13 +1359,13 @@
       <c r="E64"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
       <c r="E65"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
       <c r="E66"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
@@ -1378,33 +1375,33 @@
       <c r="E68"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="44"/>
-      <c r="C69" s="45"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="25"/>
       <c r="E69"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="44"/>
-      <c r="C70" s="45"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
       <c r="E70"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="44"/>
-      <c r="C71" s="45"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="25"/>
       <c r="E71"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="44"/>
-      <c r="C72" s="45"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="25"/>
       <c r="E72"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="44"/>
-      <c r="C73" s="45"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
       <c r="E73"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="44"/>
-      <c r="C74" s="45"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="25"/>
       <c r="E74"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -1414,23 +1411,23 @@
       <c r="E76"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="25"/>
       <c r="E77"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
       <c r="E78"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="44"/>
-      <c r="C79" s="45"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
       <c r="E79"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="44"/>
-      <c r="C80" s="45"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
       <c r="E80"/>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
@@ -1940,32 +1937,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="38">
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A4:E5"/>
     <mergeCell ref="A6:E7"/>
     <mergeCell ref="E11:H11"/>
@@ -1978,6 +1949,32 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fixing data dan struktur organisasi tag nya belum nutup dengan betul
</commit_message>
<xml_diff>
--- a/public/template/Template_Dirjab.xlsx
+++ b/public/template/Template_Dirjab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\DIRJAB-IP\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA6411E-0D70-467E-AED9-B766073B7613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB8939D-D00B-4EED-BFA9-0C3B00617371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -400,11 +400,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -452,67 +461,77 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56:H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -944,56 +963,56 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="43"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -1006,15 +1025,15 @@
     </row>
     <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
@@ -1024,29 +1043,29 @@
       <c r="D11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="s">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="44"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
@@ -1054,14 +1073,14 @@
       <c r="D13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-    </row>
-    <row r="14" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1069,14 +1088,14 @@
       <c r="D14" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-    </row>
-    <row r="15" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
@@ -1084,12 +1103,12 @@
       <c r="D15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
@@ -1099,12 +1118,12 @@
       <c r="D16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-    </row>
-    <row r="17" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>19</v>
       </c>
@@ -1112,14 +1131,14 @@
       <c r="D17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:8" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>21</v>
       </c>
@@ -1127,12 +1146,12 @@
       <c r="D18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
@@ -1144,26 +1163,26 @@
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
@@ -1185,45 +1204,45 @@
     </row>
     <row r="25" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28" t="s">
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="28"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="22">
         <v>1</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33" t="s">
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="32"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28"/>
@@ -1306,33 +1325,39 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28" t="s">
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="28"/>
+      <c r="H55" s="34"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E56"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E57"/>
@@ -1359,13 +1384,13 @@
       <c r="E64"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
       <c r="E65"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="23"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
       <c r="E66"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
@@ -1375,33 +1400,33 @@
       <c r="E68"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="24"/>
-      <c r="C69" s="25"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="37"/>
       <c r="E69"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="24"/>
-      <c r="C70" s="25"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="37"/>
       <c r="E70"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="24"/>
-      <c r="C71" s="25"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="37"/>
       <c r="E71"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="24"/>
-      <c r="C72" s="25"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="37"/>
       <c r="E72"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="37"/>
       <c r="E73"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="24"/>
-      <c r="C74" s="25"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="37"/>
       <c r="E74"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
@@ -1411,23 +1436,23 @@
       <c r="E76"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="24"/>
-      <c r="C77" s="25"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="37"/>
       <c r="E77"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="37"/>
       <c r="E78"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="37"/>
       <c r="E79"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="37"/>
       <c r="E80"/>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
@@ -1936,30 +1961,9 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="38">
-    <mergeCell ref="A4:E5"/>
-    <mergeCell ref="A6:E7"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:H27"/>
+  <mergeCells count="40">
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="G56:H56"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B54:H54"/>
@@ -1975,6 +1979,29 @@
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="B71:C71"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="A4:E5"/>
+    <mergeCell ref="A6:E7"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>